<commit_message>
Template orientation update, with logo
</commit_message>
<xml_diff>
--- a/API/Model/GenerateExcel/Templates/Attainment Timeline.xlsx
+++ b/API/Model/GenerateExcel/Templates/Attainment Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GC-FaMS-API\API\Model\GenerateExcel\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82A647D-8CFD-4397-97FF-0ACD607295EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE6E819-9593-4526-B206-2AC6B611C9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{9BFB484B-CCF6-4471-8DB9-57ECD0265C47}"/>
+    <workbookView xWindow="29625" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{9BFB484B-CCF6-4471-8DB9-57ECD0265C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -194,6 +194,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>623455</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>33312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F79EA73-57E3-2D52-E331-10E27C45C154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1801091" cy="1799767"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -522,21 +577,21 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="43.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -547,7 +602,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -560,7 +615,7 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -571,7 +626,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="25.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -582,7 +637,7 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="8" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -611,7 +666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -622,7 +677,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -633,7 +688,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -644,7 +699,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -655,7 +710,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -666,7 +721,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -677,7 +732,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -688,7 +743,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -699,7 +754,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -710,7 +765,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -721,7 +776,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -732,7 +787,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -743,7 +798,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -754,7 +809,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -765,7 +820,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -776,7 +831,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -787,7 +842,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -805,6 +860,7 @@
     <mergeCell ref="A6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="46" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>